<commit_message>
update test excel files;
</commit_message>
<xml_diff>
--- a/swiftboot-sheet/src/test/resources/exp/template.xlsx
+++ b/swiftboot-sheet/src/test/resources/exp/template.xlsx
@@ -158,7 +158,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,6 +196,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -282,9 +286,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>547200</xdr:colOff>
+      <xdr:colOff>546840</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>489960</xdr:rowOff>
+      <xdr:rowOff>489600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -298,7 +302,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="547200" cy="489960"/>
+          <a:ext cx="546840" cy="489600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -324,9 +328,9 @@
       <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.95"/>
   </cols>
@@ -531,8 +535,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -543,20 +547,216 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
+      <selection pane="topLeft" activeCell="R14" activeCellId="0" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>